<commit_message>
Update Vendor Portal Excel template
Replaces the existing Vendor_Portal_Template.xlsx file with a new version. The update may include changes to the template's structure, formatting, or data to better support vendor portal requirements.
</commit_message>
<xml_diff>
--- a/public/Vendor_Portal_Template.xlsx
+++ b/public/Vendor_Portal_Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\64638\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE8391A5-C54F-4216-B0F1-976169623ECA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E2CC935-165E-422B-9BE1-4C296A73117D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F1B74D70-85CD-DC4F-9DE8-ED882C010349}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="131">
   <si>
     <t>UPC</t>
   </si>
@@ -359,10 +359,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Vendor SKU</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Harmonized #</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -432,6 +428,14 @@
   </si>
   <si>
     <t>Damaged</t>
+  </si>
+  <si>
+    <t>SD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SKU</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -859,348 +863,370 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{508C27F0-AEB8-F043-B982-1633E0AECFA0}">
-  <dimension ref="A1:DE2"/>
+  <dimension ref="A1:DL2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="CH1" workbookViewId="0">
+      <selection activeCell="CT7" sqref="CT7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="13.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:116" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="M1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="O1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>6</v>
+      </c>
+      <c r="R1" t="s">
+        <v>7</v>
+      </c>
+      <c r="S1" t="s">
+        <v>8</v>
+      </c>
+      <c r="T1" t="s">
+        <v>9</v>
+      </c>
+      <c r="U1" t="s">
+        <v>10</v>
+      </c>
+      <c r="V1" t="s">
+        <v>11</v>
+      </c>
+      <c r="W1" t="s">
+        <v>12</v>
+      </c>
+      <c r="X1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AE1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>40</v>
+      </c>
+      <c r="BA1" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K1" t="s">
-        <v>7</v>
-      </c>
-      <c r="L1" t="s">
-        <v>8</v>
-      </c>
-      <c r="M1" t="s">
-        <v>9</v>
-      </c>
-      <c r="N1" t="s">
-        <v>10</v>
-      </c>
-      <c r="O1" t="s">
-        <v>11</v>
-      </c>
-      <c r="P1" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>13</v>
-      </c>
-      <c r="R1" t="s">
-        <v>14</v>
-      </c>
-      <c r="S1" t="s">
-        <v>15</v>
-      </c>
-      <c r="T1" t="s">
-        <v>16</v>
-      </c>
-      <c r="U1" t="s">
-        <v>17</v>
-      </c>
-      <c r="V1" t="s">
-        <v>18</v>
-      </c>
-      <c r="W1" t="s">
-        <v>19</v>
-      </c>
-      <c r="X1" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>21</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>23</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>108</v>
-      </c>
-      <c r="AS1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AT1" t="s">
-        <v>107</v>
-      </c>
-      <c r="AU1" t="s">
+      <c r="BB1" t="s">
         <v>41</v>
       </c>
-      <c r="AV1" s="4" t="s">
+      <c r="BC1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="AW1" s="4" t="s">
+      <c r="BD1" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="AX1" s="4" t="s">
+      <c r="BE1" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="AY1" s="4" t="s">
+      <c r="BF1" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="AZ1" s="4" t="s">
+      <c r="BG1" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="BA1" s="4" t="s">
+      <c r="BH1" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="BB1" s="4" t="s">
+      <c r="BI1" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="BC1" s="4" t="s">
+      <c r="BJ1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BK1" t="s">
         <v>50</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BL1" t="s">
         <v>51</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BM1" t="s">
         <v>52</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BN1" t="s">
         <v>53</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BO1" t="s">
         <v>54</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BP1" t="s">
         <v>55</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BQ1" t="s">
         <v>56</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="BR1" t="s">
         <v>57</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="BS1" t="s">
         <v>58</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="BT1" t="s">
         <v>59</v>
       </c>
-      <c r="BN1" t="s">
+      <c r="BU1" t="s">
         <v>60</v>
       </c>
-      <c r="BO1" t="s">
+      <c r="BV1" t="s">
         <v>61</v>
       </c>
-      <c r="BP1" t="s">
+      <c r="BW1" t="s">
         <v>62</v>
       </c>
-      <c r="BQ1" t="s">
+      <c r="BX1" t="s">
         <v>63</v>
       </c>
-      <c r="BR1" t="s">
+      <c r="BY1" t="s">
         <v>64</v>
       </c>
-      <c r="BS1" t="s">
+      <c r="BZ1" t="s">
         <v>65</v>
       </c>
-      <c r="BT1" t="s">
+      <c r="CA1" t="s">
         <v>66</v>
       </c>
-      <c r="BU1" t="s">
+      <c r="CB1" t="s">
         <v>67</v>
       </c>
-      <c r="BV1" t="s">
+      <c r="CC1" t="s">
         <v>68</v>
       </c>
-      <c r="BW1" t="s">
+      <c r="CD1" t="s">
         <v>69</v>
       </c>
-      <c r="BX1" t="s">
+      <c r="CE1" t="s">
         <v>70</v>
       </c>
-      <c r="BY1" t="s">
+      <c r="CF1" t="s">
         <v>71</v>
       </c>
-      <c r="BZ1" t="s">
+      <c r="CG1" t="s">
         <v>72</v>
       </c>
-      <c r="CA1" t="s">
+      <c r="CH1" t="s">
         <v>73</v>
       </c>
-      <c r="CB1" t="s">
+      <c r="CI1" t="s">
         <v>74</v>
       </c>
-      <c r="CC1" t="s">
+      <c r="CJ1" t="s">
         <v>75</v>
       </c>
-      <c r="CD1" t="s">
+      <c r="CK1" t="s">
         <v>76</v>
       </c>
-      <c r="CE1" t="s">
+      <c r="CL1" t="s">
         <v>77</v>
       </c>
-      <c r="CF1" s="4" t="s">
+      <c r="CM1" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="CG1" t="s">
+      <c r="CN1" t="s">
         <v>79</v>
       </c>
-      <c r="CH1" t="s">
+      <c r="CO1" t="s">
         <v>80</v>
       </c>
-      <c r="CI1" t="s">
+      <c r="CP1" t="s">
         <v>81</v>
       </c>
-      <c r="CJ1" t="s">
+      <c r="CQ1" t="s">
         <v>82</v>
       </c>
-      <c r="CK1" t="s">
+      <c r="CR1" t="s">
         <v>83</v>
       </c>
-      <c r="CL1" t="s">
+      <c r="CS1" t="s">
         <v>84</v>
       </c>
-      <c r="CM1" s="4" t="s">
+      <c r="CT1" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="CN1" t="s">
+      <c r="CU1" t="s">
         <v>85</v>
       </c>
-      <c r="CO1" t="s">
+      <c r="CV1" t="s">
         <v>86</v>
       </c>
-      <c r="CP1" t="s">
+      <c r="CW1" t="s">
         <v>87</v>
       </c>
-      <c r="CQ1" t="s">
+      <c r="CX1" t="s">
         <v>88</v>
       </c>
-      <c r="CR1" t="s">
+      <c r="CY1" t="s">
         <v>89</v>
       </c>
-      <c r="CS1" t="s">
+      <c r="CZ1" t="s">
         <v>90</v>
       </c>
-      <c r="CT1" t="s">
+      <c r="DA1" t="s">
         <v>91</v>
       </c>
-      <c r="CU1" t="s">
+      <c r="DB1" t="s">
         <v>92</v>
       </c>
-      <c r="CV1" t="s">
+      <c r="DC1" t="s">
         <v>93</v>
       </c>
-      <c r="CW1" t="s">
+      <c r="DD1" t="s">
         <v>94</v>
       </c>
-      <c r="CX1" t="s">
+      <c r="DE1" t="s">
         <v>95</v>
       </c>
-      <c r="CY1" t="s">
+      <c r="DF1" t="s">
         <v>96</v>
       </c>
-      <c r="CZ1" t="s">
+      <c r="DG1" t="s">
         <v>97</v>
       </c>
-      <c r="DA1" t="s">
+      <c r="DH1" t="s">
         <v>98</v>
       </c>
-      <c r="DB1" t="s">
+      <c r="DI1" t="s">
         <v>99</v>
       </c>
-      <c r="DC1" t="s">
+      <c r="DJ1" t="s">
         <v>100</v>
       </c>
-      <c r="DD1" t="s">
+      <c r="DK1" t="s">
         <v>101</v>
       </c>
-      <c r="DE1" t="s">
+      <c r="DL1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:109" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:116" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="G2" s="2"/>
@@ -1233,13 +1259,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>110</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1247,7 +1273,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C2" s="6" t="str">
         <f>A2 &amp; " – " &amp; B2</f>
@@ -1259,7 +1285,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C3" s="6" t="str">
         <f t="shared" ref="C3:C9" si="0">A3 &amp; " – " &amp; B3</f>
@@ -1271,7 +1297,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C4" s="6" t="str">
         <f t="shared" si="0"/>
@@ -1283,7 +1309,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C5" s="6" t="str">
         <f t="shared" si="0"/>
@@ -1295,7 +1321,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C6" s="6" t="str">
         <f t="shared" si="0"/>
@@ -1307,7 +1333,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C7" s="6" t="str">
         <f t="shared" si="0"/>
@@ -1319,7 +1345,7 @@
         <v>11</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C8" s="6" t="str">
         <f t="shared" si="0"/>
@@ -1331,7 +1357,7 @@
         <v>12</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C9" s="6" t="str">
         <f t="shared" si="0"/>
@@ -1356,13 +1382,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>121</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1370,7 +1396,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C2" s="6" t="str">
         <f>A2 &amp; " – " &amp; B2</f>
@@ -1382,7 +1408,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C3" s="6" t="str">
         <f t="shared" ref="C3:C9" si="0">A3 &amp; " – " &amp; B3</f>
@@ -1394,7 +1420,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C4" s="6" t="str">
         <f t="shared" si="0"/>
@@ -1406,7 +1432,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C5" s="6" t="str">
         <f t="shared" si="0"/>
@@ -1418,7 +1444,7 @@
         <v>8</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C6" s="6" t="str">
         <f t="shared" si="0"/>
@@ -1430,7 +1456,7 @@
         <v>9</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C7" s="6" t="str">
         <f t="shared" si="0"/>
@@ -1442,7 +1468,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C8" s="6" t="str">
         <f t="shared" si="0"/>
@@ -1454,7 +1480,7 @@
         <v>11</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C9" s="6" t="str">
         <f t="shared" si="0"/>

</xml_diff>